<commit_message>
add(import): Add imports inventory
</commit_message>
<xml_diff>
--- a/model-excel-import/inventaries.xlsx
+++ b/model-excel-import/inventaries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ei-sistema\model-excel-import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B6ED3E-9C18-4996-A885-C8A9A0524DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F2FA9A-1799-4F11-AB4F-0D2F7430FC15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="5295" windowWidth="15375" windowHeight="8415" xr2:uid="{7668B1A8-A5AD-44CF-B6D1-FD20371924DB}"/>
+    <workbookView xWindow="8430" yWindow="2760" windowWidth="18165" windowHeight="12255" xr2:uid="{7668B1A8-A5AD-44CF-B6D1-FD20371924DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,29 +25,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>nombre</t>
   </si>
   <si>
-    <t>codigo</t>
-  </si>
-  <si>
     <t>tipo</t>
   </si>
   <si>
-    <t>modelo</t>
-  </si>
-  <si>
     <t>cantidad</t>
   </si>
   <si>
     <t>estado</t>
   </si>
   <si>
-    <t>descripcion</t>
-  </si>
-  <si>
     <t>unidad</t>
   </si>
   <si>
@@ -87,21 +78,29 @@
     <t>Equipos informáticos</t>
   </si>
   <si>
-    <t>Computadora marca Dell</t>
-  </si>
-  <si>
-    <t>Inspiron</t>
-  </si>
-  <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>codigo_partida</t>
+  </si>
+  <si>
+    <t>codigo_catalogo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,7 +130,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,122 +445,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDAC11A1-B206-40DA-A1CF-B3B3DD13143E}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="1"/>
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
       <c r="E2">
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>18</v>
       </c>
       <c r="E3">
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
       </c>
       <c r="E4">
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E5">
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
add(inventory): Add export in excel and pdf and import in excel
</commit_message>
<xml_diff>
--- a/model-excel-import/inventaries.xlsx
+++ b/model-excel-import/inventaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ei-sistema\model-excel-import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{300A0EE0-A18F-4404-9DD6-BE48D28CFA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFB6E5D-F352-4308-8988-5AF8F6121261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8430" yWindow="2760" windowWidth="18165" windowHeight="12255" xr2:uid="{7668B1A8-A5AD-44CF-B6D1-FD20371924DB}"/>
+    <workbookView xWindow="9825" yWindow="2055" windowWidth="18120" windowHeight="12255" xr2:uid="{7668B1A8-A5AD-44CF-B6D1-FD20371924DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>nombre</t>
   </si>
@@ -33,12 +33,6 @@
     <t>tipo</t>
   </si>
   <si>
-    <t>cantidad</t>
-  </si>
-  <si>
-    <t>unidad</t>
-  </si>
-  <si>
     <t>FC51</t>
   </si>
   <si>
@@ -76,6 +70,15 @@
   </si>
   <si>
     <t>codigo_catalogo</t>
+  </si>
+  <si>
+    <t>descripcion</t>
+  </si>
+  <si>
+    <t>cantidad_contenedor</t>
+  </si>
+  <si>
+    <t>unidades_contenedor</t>
   </si>
 </sst>
 </file>
@@ -439,22 +442,24 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="15.28515625" customWidth="1"/>
     <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -463,81 +468,102 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="F1" t="s">
-        <v>3</v>
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
-        <v>12</v>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3">
+      <c r="G3">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>